<commit_message>
finished bom and schematic - nano
</commit_message>
<xml_diff>
--- a/micro/EDA/microBoSL BOM Rev 0.1.0.xlsx
+++ b/micro/EDA/microBoSL BOM Rev 0.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Repositories\BoSL-nano\micro\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FAD1A3-CCA0-4C0B-8521-7156BF963009}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934522B8-FAB8-491E-A02E-BAB08E503C26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,7 +726,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -815,7 +815,7 @@
         <v>0.1</v>
       </c>
       <c r="H3" s="13">
-        <f t="shared" ref="H3:H28" si="0">F3*G3</f>
+        <f t="shared" ref="H3:H20" si="0">F3*G3</f>
         <v>0.2</v>
       </c>
       <c r="I3" s="5"/>

</xml_diff>